<commit_message>
commit adição de 41 novos pacientes
</commit_message>
<xml_diff>
--- a/SINTOMAS CORONAVIRUS.xlsx
+++ b/SINTOMAS CORONAVIRUS.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1588791772" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1588791772" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1588791772" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1588791772"/>
+      <pm:revision xmlns:pm="smNativeData" day="1588954570" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1588954570" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1588954570" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1588954570"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="191">
   <si>
     <t>CORONAVIRUS</t>
   </si>
@@ -518,13 +518,91 @@
   </si>
   <si>
     <t>16, 20</t>
+  </si>
+  <si>
+    <t>10, 16, 18, 20, 21</t>
+  </si>
+  <si>
+    <t>14, 10, 16, 20, 21</t>
+  </si>
+  <si>
+    <t>10, 12, 16, 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10, 20, 21</t>
+  </si>
+  <si>
+    <t>10, 11, 20, 21</t>
+  </si>
+  <si>
+    <t>14, 12, 20, 21, 26</t>
+  </si>
+  <si>
+    <t>20, 21, 12</t>
+  </si>
+  <si>
+    <t>15, 21, 20</t>
+  </si>
+  <si>
+    <t>10, 12, 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 21, 15, 23 </t>
+  </si>
+  <si>
+    <t>21, 13, 15</t>
+  </si>
+  <si>
+    <t>22, 21, 12, 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21, 12, 20</t>
+  </si>
+  <si>
+    <t>20, 13, 21, 14</t>
+  </si>
+  <si>
+    <t>10, 12, 20, 21, 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10, 15, 20</t>
+  </si>
+  <si>
+    <t>10, 14, 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 20, 21 </t>
+  </si>
+  <si>
+    <t>14, 21, 22</t>
+  </si>
+  <si>
+    <t>24, 11, 13, 14, 10, 20, 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10, 21</t>
+  </si>
+  <si>
+    <t>14, 12, 21, 20</t>
+  </si>
+  <si>
+    <t>16, 18, 20, 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10, 14, 21</t>
+  </si>
+  <si>
+    <t>11, 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12, 20, 21, 26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -533,7 +611,6 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="MM/DD/YY h"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -543,7 +620,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1588791772" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1588954570" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -559,7 +636,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1588791772" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1588954570" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -593,7 +670,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -604,7 +681,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -615,7 +692,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -626,7 +703,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -640,7 +717,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -657,7 +734,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -680,7 +757,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -691,7 +768,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -702,7 +779,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -725,7 +802,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -736,7 +813,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -774,7 +851,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -785,7 +862,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -802,7 +879,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588791772" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -842,7 +919,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772"/>
+          <pm:border xmlns:pm="smNativeData" id="1588954570"/>
         </ext>
       </extLst>
     </border>
@@ -861,7 +938,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -885,7 +962,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -909,7 +986,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -932,7 +1009,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -954,7 +1031,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -978,7 +1055,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1002,7 +1079,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1026,7 +1103,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1050,7 +1127,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1073,7 +1150,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1097,7 +1174,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1120,7 +1197,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1144,7 +1221,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1168,7 +1245,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1191,7 +1268,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1215,7 +1292,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1239,7 +1316,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1263,7 +1340,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1286,7 +1363,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1309,7 +1386,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1332,7 +1409,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1356,7 +1433,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1380,7 +1457,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1404,7 +1481,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1427,7 +1504,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1450,7 +1527,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1473,7 +1550,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1496,7 +1573,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1517,7 +1594,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1540,7 +1617,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1564,7 +1641,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1588,7 +1665,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1611,7 +1688,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1633,7 +1710,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1656,7 +1733,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1680,7 +1757,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1703,7 +1780,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1726,7 +1803,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1749,7 +1826,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1771,7 +1848,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772"/>
+          <pm:border xmlns:pm="smNativeData" id="1588954570"/>
         </ext>
       </extLst>
     </border>
@@ -1790,7 +1867,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1812,7 +1889,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1833,7 +1910,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1854,7 +1931,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1876,7 +1953,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1897,7 +1974,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588791772">
+          <pm:border xmlns:pm="smNativeData" id="1588954570">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -2109,10 +2186,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1588791772" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1588954570" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1588791772" count="4">
+      <pm:colors xmlns:pm="smNativeData" id="1588954570" count="4">
         <pm:color name="Color 24" rgb="FFFF9E"/>
         <pm:color name="Color 25" rgb="FF9E9E"/>
         <pm:color name="Color 26" rgb="FFFFE0"/>
@@ -2379,15 +2456,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H305"/>
+  <dimension ref="A1:H346"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F290" sqref="F290"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="16384" width="20.405405" customWidth="1"/>
+    <col min="1" max="3" width="20.405405" customWidth="1"/>
+    <col min="4" max="4" width="21.216216" customWidth="1"/>
+    <col min="5" max="16384" width="20.405405" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4998,13 +5077,13 @@
       <c r="A161" s="40" t="n">
         <v>126</v>
       </c>
-      <c r="B161" s="63" t="n">
+      <c r="B161" s="12" t="n">
         <v>25</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D161" s="63" t="s">
+      <c r="D161" s="12" t="s">
         <v>120</v>
       </c>
       <c r="E161" s="66" t="s">
@@ -5015,13 +5094,13 @@
       <c r="A162" s="40" t="n">
         <v>127</v>
       </c>
-      <c r="B162" s="63" t="n">
+      <c r="B162" s="12" t="n">
         <v>25</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D162" s="63" t="s">
+      <c r="D162" s="12" t="s">
         <v>121</v>
       </c>
       <c r="E162" s="66" t="s">
@@ -5032,13 +5111,13 @@
       <c r="A163" s="40" t="n">
         <v>128</v>
       </c>
-      <c r="B163" s="63" t="n">
+      <c r="B163" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C163" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D163" s="63" t="s">
+      <c r="C163" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D163" s="12" t="s">
         <v>122</v>
       </c>
       <c r="E163" s="66" t="s">
@@ -5049,13 +5128,13 @@
       <c r="A164" s="40" t="n">
         <v>129</v>
       </c>
-      <c r="B164" s="63" t="n">
+      <c r="B164" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C164" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D164" s="63" t="n">
+      <c r="C164" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D164" s="12" t="n">
         <v>18</v>
       </c>
       <c r="E164" s="66" t="s">
@@ -5066,13 +5145,13 @@
       <c r="A165" s="40" t="n">
         <v>130</v>
       </c>
-      <c r="B165" s="63" t="n">
+      <c r="B165" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D165" s="63" t="n">
+      <c r="D165" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E165" s="66" t="s">
@@ -5083,13 +5162,13 @@
       <c r="A166" s="40" t="n">
         <v>131</v>
       </c>
-      <c r="B166" s="63" t="n">
+      <c r="B166" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D166" s="63" t="n">
+      <c r="D166" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E166" s="66" t="s">
@@ -5100,13 +5179,13 @@
       <c r="A167" s="40" t="n">
         <v>132</v>
       </c>
-      <c r="B167" s="63" t="n">
+      <c r="B167" s="12" t="n">
         <v>75</v>
       </c>
       <c r="C167" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D167" s="63" t="n">
+      <c r="D167" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E167" s="66" t="s">
@@ -5117,13 +5196,13 @@
       <c r="A168" s="40" t="n">
         <v>133</v>
       </c>
-      <c r="B168" s="63" t="n">
+      <c r="B168" s="12" t="n">
         <v>75</v>
       </c>
       <c r="C168" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D168" s="63" t="s">
+      <c r="D168" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E168" s="66" t="s">
@@ -5134,13 +5213,13 @@
       <c r="A169" s="40" t="n">
         <v>134</v>
       </c>
-      <c r="B169" s="63" t="n">
+      <c r="B169" s="12" t="n">
         <v>45</v>
       </c>
       <c r="C169" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D169" s="63" t="s">
+      <c r="D169" s="12" t="s">
         <v>123</v>
       </c>
       <c r="E169" s="66" t="s">
@@ -5151,13 +5230,13 @@
       <c r="A170" s="40" t="n">
         <v>135</v>
       </c>
-      <c r="B170" s="63" t="n">
+      <c r="B170" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C170" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D170" s="63" t="n">
+      <c r="C170" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D170" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E170" s="66" t="s">
@@ -5168,13 +5247,13 @@
       <c r="A171" s="40" t="n">
         <v>136</v>
       </c>
-      <c r="B171" s="63" t="n">
+      <c r="B171" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C171" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D171" s="63" t="n">
+      <c r="C171" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D171" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E171" s="66" t="s">
@@ -5185,13 +5264,13 @@
       <c r="A172" s="40" t="n">
         <v>137</v>
       </c>
-      <c r="B172" s="63" t="n">
+      <c r="B172" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C172" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D172" s="63" t="n">
+      <c r="C172" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D172" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E172" s="66" t="s">
@@ -5202,13 +5281,13 @@
       <c r="A173" s="40" t="n">
         <v>138</v>
       </c>
-      <c r="B173" s="63" t="n">
+      <c r="B173" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="C173" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D173" s="63" t="s">
+      <c r="C173" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D173" s="12" t="s">
         <v>124</v>
       </c>
       <c r="E173" s="66" t="s">
@@ -5219,13 +5298,13 @@
       <c r="A174" s="40" t="n">
         <v>139</v>
       </c>
-      <c r="B174" s="63" t="n">
+      <c r="B174" s="12" t="n">
         <v>25</v>
       </c>
       <c r="C174" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D174" s="63" t="s">
+      <c r="D174" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E174" s="66" t="s">
@@ -5236,13 +5315,13 @@
       <c r="A175" s="40" t="n">
         <v>140</v>
       </c>
-      <c r="B175" s="63" t="n">
+      <c r="B175" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C175" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D175" s="63" t="n">
+      <c r="C175" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D175" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E175" s="66" t="s">
@@ -5253,13 +5332,13 @@
       <c r="A176" s="40" t="n">
         <v>141</v>
       </c>
-      <c r="B176" s="63" t="n">
+      <c r="B176" s="12" t="n">
         <v>75</v>
       </c>
       <c r="C176" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D176" s="63" t="s">
+      <c r="D176" s="12" t="s">
         <v>125</v>
       </c>
       <c r="E176" s="66" t="s">
@@ -5270,13 +5349,13 @@
       <c r="A177" s="40" t="n">
         <v>142</v>
       </c>
-      <c r="B177" s="63" t="n">
+      <c r="B177" s="12" t="n">
         <v>75</v>
       </c>
       <c r="C177" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D177" s="63" t="s">
+      <c r="D177" s="12" t="s">
         <v>108</v>
       </c>
       <c r="E177" s="66" t="s">
@@ -5287,13 +5366,13 @@
       <c r="A178" s="40" t="n">
         <v>143</v>
       </c>
-      <c r="B178" s="63" t="n">
+      <c r="B178" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C178" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D178" s="63" t="s">
+      <c r="C178" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D178" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E178" s="66" t="s">
@@ -5304,13 +5383,13 @@
       <c r="A179" s="40" t="n">
         <v>144</v>
       </c>
-      <c r="B179" s="63" t="n">
+      <c r="B179" s="12" t="n">
         <v>45</v>
       </c>
       <c r="C179" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D179" s="63" t="s">
+      <c r="D179" s="12" t="s">
         <v>126</v>
       </c>
       <c r="E179" s="66" t="s">
@@ -5321,13 +5400,13 @@
       <c r="A180" s="40" t="n">
         <v>145</v>
       </c>
-      <c r="B180" s="63" t="n">
+      <c r="B180" s="12" t="n">
         <v>85</v>
       </c>
-      <c r="C180" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D180" s="63" t="s">
+      <c r="C180" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D180" s="12" t="s">
         <v>127</v>
       </c>
       <c r="E180" s="66" t="s">
@@ -5338,13 +5417,13 @@
       <c r="A181" s="40" t="n">
         <v>146</v>
       </c>
-      <c r="B181" s="63" t="n">
+      <c r="B181" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C181" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D181" s="63" t="s">
+      <c r="C181" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D181" s="12" t="s">
         <v>127</v>
       </c>
       <c r="E181" s="66" t="s">
@@ -5355,13 +5434,13 @@
       <c r="A182" s="40" t="n">
         <v>147</v>
       </c>
-      <c r="B182" s="63" t="n">
+      <c r="B182" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C182" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D182" s="63" t="s">
+      <c r="C182" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D182" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E182" s="66" t="s">
@@ -5372,13 +5451,13 @@
       <c r="A183" s="40" t="n">
         <v>148</v>
       </c>
-      <c r="B183" s="63" t="n">
+      <c r="B183" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C183" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D183" s="63" t="s">
+      <c r="C183" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D183" s="12" t="s">
         <v>106</v>
       </c>
       <c r="E183" s="66" t="s">
@@ -5389,13 +5468,13 @@
       <c r="A184" s="40" t="n">
         <v>149</v>
       </c>
-      <c r="B184" s="63" t="n">
+      <c r="B184" s="12" t="n">
         <v>75</v>
       </c>
       <c r="C184" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D184" s="63" t="s">
+      <c r="D184" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E184" s="66" t="s">
@@ -5406,13 +5485,13 @@
       <c r="A185" s="40" t="n">
         <v>150</v>
       </c>
-      <c r="B185" s="63" t="n">
+      <c r="B185" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C185" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D185" s="63" t="s">
+      <c r="C185" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D185" s="12" t="s">
         <v>129</v>
       </c>
       <c r="E185" s="66" t="s">
@@ -5423,13 +5502,13 @@
       <c r="A186" s="40" t="n">
         <v>151</v>
       </c>
-      <c r="B186" s="63" t="n">
+      <c r="B186" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C186" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D186" s="63" t="s">
+      <c r="D186" s="12" t="s">
         <v>130</v>
       </c>
       <c r="E186" s="66" t="s">
@@ -5440,13 +5519,13 @@
       <c r="A187" s="40" t="n">
         <v>152</v>
       </c>
-      <c r="B187" s="63" t="n">
+      <c r="B187" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C187" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D187" s="63" t="n">
+      <c r="C187" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D187" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E187" s="66" t="s">
@@ -5457,13 +5536,13 @@
       <c r="A188" s="40" t="n">
         <v>153</v>
       </c>
-      <c r="B188" s="63" t="n">
+      <c r="B188" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C188" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D188" s="63" t="s">
+      <c r="C188" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D188" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E188" s="66" t="s">
@@ -5474,13 +5553,13 @@
       <c r="A189" s="40" t="n">
         <v>154</v>
       </c>
-      <c r="B189" s="63" t="n">
+      <c r="B189" s="12" t="n">
         <v>60</v>
       </c>
       <c r="C189" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D189" s="63" t="s">
+      <c r="D189" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E189" s="66" t="s">
@@ -5491,13 +5570,13 @@
       <c r="A190" s="40" t="n">
         <v>155</v>
       </c>
-      <c r="B190" s="63" t="n">
+      <c r="B190" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C190" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D190" s="63" t="s">
+      <c r="C190" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D190" s="12" t="s">
         <v>131</v>
       </c>
       <c r="E190" s="66" t="s">
@@ -5508,13 +5587,13 @@
       <c r="A191" s="40" t="n">
         <v>156</v>
       </c>
-      <c r="B191" s="63" t="n">
+      <c r="B191" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C191" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D191" s="63" t="s">
+      <c r="C191" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D191" s="12" t="s">
         <v>132</v>
       </c>
       <c r="E191" s="66" t="s">
@@ -5525,13 +5604,13 @@
       <c r="A192" s="40" t="n">
         <v>157</v>
       </c>
-      <c r="B192" s="63" t="n">
+      <c r="B192" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="C192" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D192" s="63" t="n">
+      <c r="C192" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D192" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E192" s="66" t="s">
@@ -5542,13 +5621,13 @@
       <c r="A193" s="40" t="n">
         <v>158</v>
       </c>
-      <c r="B193" s="63" t="n">
+      <c r="B193" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C193" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D193" s="63" t="s">
+      <c r="C193" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D193" s="12" t="s">
         <v>122</v>
       </c>
       <c r="E193" s="66" t="s">
@@ -5559,13 +5638,13 @@
       <c r="A194" s="40" t="n">
         <v>159</v>
       </c>
-      <c r="B194" s="63" t="n">
+      <c r="B194" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C194" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D194" s="63" t="s">
+      <c r="C194" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D194" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E194" s="66" t="s">
@@ -5576,13 +5655,13 @@
       <c r="A195" s="40" t="n">
         <v>160</v>
       </c>
-      <c r="B195" s="63" t="n">
+      <c r="B195" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C195" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D195" s="63" t="s">
+      <c r="C195" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D195" s="12" t="s">
         <v>134</v>
       </c>
       <c r="E195" s="66" t="s">
@@ -5593,13 +5672,13 @@
       <c r="A196" s="40" t="n">
         <v>161</v>
       </c>
-      <c r="B196" s="63" t="n">
+      <c r="B196" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C196" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D196" s="63" t="n">
+      <c r="C196" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D196" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E196" s="66" t="s">
@@ -5610,13 +5689,13 @@
       <c r="A197" s="40" t="n">
         <v>162</v>
       </c>
-      <c r="B197" s="63" t="n">
+      <c r="B197" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C197" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D197" s="63" t="s">
+      <c r="C197" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D197" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E197" s="66" t="s">
@@ -5627,13 +5706,13 @@
       <c r="A198" s="40" t="n">
         <v>163</v>
       </c>
-      <c r="B198" s="63" t="n">
+      <c r="B198" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="C198" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D198" s="63" t="s">
+      <c r="C198" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D198" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E198" s="66" t="s">
@@ -5644,13 +5723,13 @@
       <c r="A199" s="40" t="n">
         <v>164</v>
       </c>
-      <c r="B199" s="63" t="n">
+      <c r="B199" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C199" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D199" s="63" t="s">
+      <c r="C199" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D199" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E199" s="66" t="s">
@@ -5661,13 +5740,13 @@
       <c r="A200" s="40" t="n">
         <v>165</v>
       </c>
-      <c r="B200" s="63" t="n">
+      <c r="B200" s="12" t="n">
         <v>85</v>
       </c>
-      <c r="C200" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D200" s="63" t="s">
+      <c r="C200" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D200" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E200" s="66" t="s">
@@ -5678,13 +5757,13 @@
       <c r="A201" s="40" t="n">
         <v>166</v>
       </c>
-      <c r="B201" s="63" t="n">
+      <c r="B201" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="C201" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D201" s="63" t="s">
+      <c r="C201" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D201" s="12" t="s">
         <v>135</v>
       </c>
       <c r="E201" s="66" t="s">
@@ -5695,13 +5774,13 @@
       <c r="A202" s="40" t="n">
         <v>167</v>
       </c>
-      <c r="B202" s="63" t="n">
+      <c r="B202" s="12" t="n">
         <v>85</v>
       </c>
-      <c r="C202" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D202" s="63" t="s">
+      <c r="C202" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D202" s="12" t="s">
         <v>136</v>
       </c>
       <c r="E202" s="66" t="s">
@@ -5712,13 +5791,13 @@
       <c r="A203" s="40" t="n">
         <v>168</v>
       </c>
-      <c r="B203" s="63" t="n">
+      <c r="B203" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C203" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D203" s="63" t="s">
+      <c r="C203" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D203" s="12" t="s">
         <v>137</v>
       </c>
       <c r="E203" s="66" t="s">
@@ -5729,13 +5808,13 @@
       <c r="A204" s="40" t="n">
         <v>169</v>
       </c>
-      <c r="B204" s="63" t="n">
+      <c r="B204" s="12" t="n">
         <v>45</v>
       </c>
       <c r="C204" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="63" t="s">
+      <c r="D204" s="12" t="s">
         <v>138</v>
       </c>
       <c r="E204" s="66" t="s">
@@ -5746,13 +5825,13 @@
       <c r="A205" s="40" t="n">
         <v>170</v>
       </c>
-      <c r="B205" s="63" t="n">
+      <c r="B205" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C205" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="63" t="n">
+      <c r="D205" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E205" s="66" t="s">
@@ -5763,13 +5842,13 @@
       <c r="A206" s="40" t="n">
         <v>171</v>
       </c>
-      <c r="B206" s="63" t="n">
+      <c r="B206" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C206" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D206" s="63" t="s">
+      <c r="C206" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D206" s="12" t="s">
         <v>139</v>
       </c>
       <c r="E206" s="66" t="s">
@@ -5780,13 +5859,13 @@
       <c r="A207" s="40" t="n">
         <v>172</v>
       </c>
-      <c r="B207" s="63" t="n">
+      <c r="B207" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="C207" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D207" s="63" t="n">
+      <c r="C207" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D207" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E207" s="66" t="s">
@@ -5797,13 +5876,13 @@
       <c r="A208" s="40" t="n">
         <v>173</v>
       </c>
-      <c r="B208" s="63" t="n">
+      <c r="B208" s="12" t="n">
         <v>40</v>
       </c>
       <c r="C208" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D208" s="63" t="s">
+      <c r="D208" s="12" t="s">
         <v>140</v>
       </c>
       <c r="E208" s="66" t="s">
@@ -5814,13 +5893,13 @@
       <c r="A209" s="40" t="n">
         <v>174</v>
       </c>
-      <c r="B209" s="63" t="n">
+      <c r="B209" s="12" t="n">
         <v>59</v>
       </c>
       <c r="C209" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D209" s="63" t="n">
+      <c r="D209" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E209" s="66" t="s">
@@ -5831,13 +5910,13 @@
       <c r="A210" s="40" t="n">
         <v>175</v>
       </c>
-      <c r="B210" s="63" t="n">
+      <c r="B210" s="12" t="n">
         <v>31</v>
       </c>
-      <c r="C210" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D210" s="63" t="n">
+      <c r="C210" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D210" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E210" s="66" t="s">
@@ -5848,13 +5927,13 @@
       <c r="A211" s="40" t="n">
         <v>176</v>
       </c>
-      <c r="B211" s="63" t="n">
+      <c r="B211" s="12" t="n">
         <v>27</v>
       </c>
-      <c r="C211" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D211" s="63" t="n">
+      <c r="C211" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D211" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E211" s="66" t="s">
@@ -5865,13 +5944,13 @@
       <c r="A212" s="40" t="n">
         <v>177</v>
       </c>
-      <c r="B212" s="63" t="n">
+      <c r="B212" s="12" t="n">
         <v>32</v>
       </c>
       <c r="C212" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D212" s="63" t="n">
+      <c r="D212" s="12" t="n">
         <v>18</v>
       </c>
       <c r="E212" s="66" t="s">
@@ -5882,13 +5961,13 @@
       <c r="A213" s="40" t="n">
         <v>178</v>
       </c>
-      <c r="B213" s="63" t="n">
+      <c r="B213" s="12" t="n">
         <v>53</v>
       </c>
       <c r="C213" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D213" s="63" t="s">
+      <c r="D213" s="12" t="s">
         <v>141</v>
       </c>
       <c r="E213" s="66" t="s">
@@ -5899,13 +5978,13 @@
       <c r="A214" s="40" t="n">
         <v>179</v>
       </c>
-      <c r="B214" s="63" t="n">
+      <c r="B214" s="12" t="n">
         <v>47</v>
       </c>
       <c r="C214" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D214" s="63" t="s">
+      <c r="D214" s="12" t="s">
         <v>142</v>
       </c>
       <c r="E214" s="66" t="s">
@@ -5916,13 +5995,13 @@
       <c r="A215" s="40" t="n">
         <v>180</v>
       </c>
-      <c r="B215" s="63" t="n">
+      <c r="B215" s="12" t="n">
         <v>47</v>
       </c>
       <c r="C215" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D215" s="63" t="n">
+      <c r="D215" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E215" s="66" t="s">
@@ -5933,13 +6012,13 @@
       <c r="A216" s="40" t="n">
         <v>181</v>
       </c>
-      <c r="B216" s="63" t="n">
+      <c r="B216" s="12" t="n">
         <v>28</v>
       </c>
       <c r="C216" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D216" s="63" t="s">
+      <c r="D216" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E216" s="66" t="s">
@@ -5950,13 +6029,13 @@
       <c r="A217" s="40" t="n">
         <v>182</v>
       </c>
-      <c r="B217" s="63" t="n">
+      <c r="B217" s="12" t="n">
         <v>41</v>
       </c>
-      <c r="C217" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D217" s="63" t="n">
+      <c r="C217" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D217" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E217" s="66" t="s">
@@ -5967,13 +6046,13 @@
       <c r="A218" s="40" t="n">
         <v>183</v>
       </c>
-      <c r="B218" s="63" t="n">
+      <c r="B218" s="12" t="n">
         <v>35</v>
       </c>
       <c r="C218" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D218" s="63" t="s">
+      <c r="D218" s="12" t="s">
         <v>143</v>
       </c>
       <c r="E218" s="66" t="s">
@@ -5984,13 +6063,13 @@
       <c r="A219" s="40" t="n">
         <v>184</v>
       </c>
-      <c r="B219" s="63" t="n">
+      <c r="B219" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C219" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D219" s="63" t="s">
+      <c r="C219" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D219" s="12" t="s">
         <v>118</v>
       </c>
       <c r="E219" s="66" t="s">
@@ -6001,13 +6080,13 @@
       <c r="A220" s="40" t="n">
         <v>185</v>
       </c>
-      <c r="B220" s="63" t="n">
-        <v>54</v>
-      </c>
-      <c r="C220" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D220" s="63" t="s">
+      <c r="B220" s="12" t="n">
+        <v>54</v>
+      </c>
+      <c r="C220" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D220" s="12" t="s">
         <v>144</v>
       </c>
       <c r="E220" s="66" t="s">
@@ -6018,13 +6097,13 @@
       <c r="A221" s="40" t="n">
         <v>186</v>
       </c>
-      <c r="B221" s="63" t="n">
+      <c r="B221" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C221" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D221" s="63" t="s">
+      <c r="C221" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D221" s="12" t="s">
         <v>145</v>
       </c>
       <c r="E221" s="66" t="s">
@@ -6035,13 +6114,13 @@
       <c r="A222" s="40" t="n">
         <v>187</v>
       </c>
-      <c r="B222" s="63" t="n">
+      <c r="B222" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="C222" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D222" s="63" t="n">
+      <c r="C222" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D222" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E222" s="66" t="s">
@@ -6052,13 +6131,13 @@
       <c r="A223" s="40" t="n">
         <v>188</v>
       </c>
-      <c r="B223" s="63" t="n">
+      <c r="B223" s="12" t="n">
         <v>52</v>
       </c>
       <c r="C223" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D223" s="63" t="n">
+      <c r="D223" s="12" t="n">
         <v>11</v>
       </c>
       <c r="E223" s="66" t="s">
@@ -6069,13 +6148,13 @@
       <c r="A224" s="40" t="n">
         <v>189</v>
       </c>
-      <c r="B224" s="63" t="n">
+      <c r="B224" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="C224" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D224" s="63" t="n">
+      <c r="C224" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D224" s="12" t="n">
         <v>13</v>
       </c>
       <c r="E224" s="66" t="s">
@@ -6086,13 +6165,13 @@
       <c r="A225" s="40" t="n">
         <v>190</v>
       </c>
-      <c r="B225" s="63" t="n">
+      <c r="B225" s="12" t="n">
         <v>42</v>
       </c>
       <c r="C225" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D225" s="63" t="n">
+      <c r="D225" s="12" t="n">
         <v>23</v>
       </c>
       <c r="E225" s="66" t="s">
@@ -6103,13 +6182,13 @@
       <c r="A226" s="40" t="n">
         <v>191</v>
       </c>
-      <c r="B226" s="63" t="n">
+      <c r="B226" s="12" t="n">
         <v>68</v>
       </c>
       <c r="C226" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D226" s="63" t="s">
+      <c r="D226" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E226" s="66" t="s">
@@ -6120,13 +6199,13 @@
       <c r="A227" s="40" t="n">
         <v>192</v>
       </c>
-      <c r="B227" s="63" t="n">
+      <c r="B227" s="12" t="n">
         <v>61</v>
       </c>
       <c r="C227" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D227" s="63" t="n">
+      <c r="D227" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E227" s="66" t="s">
@@ -6137,13 +6216,13 @@
       <c r="A228" s="40" t="n">
         <v>193</v>
       </c>
-      <c r="B228" s="63" t="n">
+      <c r="B228" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C228" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D228" s="63" t="s">
+      <c r="D228" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E228" s="66" t="s">
@@ -6154,13 +6233,13 @@
       <c r="A229" s="40" t="n">
         <v>194</v>
       </c>
-      <c r="B229" s="63" t="n">
+      <c r="B229" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C229" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D229" s="63" t="n">
+      <c r="D229" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E229" s="66" t="s">
@@ -6171,13 +6250,13 @@
       <c r="A230" s="40" t="n">
         <v>195</v>
       </c>
-      <c r="B230" s="63" t="n">
+      <c r="B230" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C230" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D230" s="63" t="s">
+      <c r="C230" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D230" s="12" t="s">
         <v>146</v>
       </c>
       <c r="E230" s="66" t="s">
@@ -6188,13 +6267,13 @@
       <c r="A231" s="40" t="n">
         <v>196</v>
       </c>
-      <c r="B231" s="63" t="n">
+      <c r="B231" s="12" t="n">
         <v>50</v>
       </c>
       <c r="C231" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D231" s="63" t="n">
+      <c r="D231" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E231" s="66" t="s">
@@ -6205,13 +6284,13 @@
       <c r="A232" s="40" t="n">
         <v>197</v>
       </c>
-      <c r="B232" s="63" t="n">
+      <c r="B232" s="12" t="n">
         <v>50</v>
       </c>
       <c r="C232" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D232" s="63" t="s">
+      <c r="D232" s="12" t="s">
         <v>147</v>
       </c>
       <c r="E232" s="66" t="s">
@@ -6222,13 +6301,13 @@
       <c r="A233" s="40" t="n">
         <v>198</v>
       </c>
-      <c r="B233" s="63" t="n">
+      <c r="B233" s="12" t="n">
         <v>70</v>
       </c>
       <c r="C233" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D233" s="63" t="n">
+      <c r="D233" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E233" s="66" t="s">
@@ -6239,13 +6318,13 @@
       <c r="A234" s="40" t="n">
         <v>199</v>
       </c>
-      <c r="B234" s="63" t="n">
+      <c r="B234" s="12" t="n">
         <v>70</v>
       </c>
       <c r="C234" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D234" s="63" t="n">
+      <c r="D234" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E234" s="66" t="s">
@@ -6256,13 +6335,13 @@
       <c r="A235" s="40" t="n">
         <v>200</v>
       </c>
-      <c r="B235" s="63" t="n">
+      <c r="B235" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C235" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D235" s="63" t="n">
+      <c r="C235" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D235" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E235" s="66" t="s">
@@ -6273,13 +6352,13 @@
       <c r="A236" s="40" t="n">
         <v>201</v>
       </c>
-      <c r="B236" s="63" t="n">
+      <c r="B236" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C236" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D236" s="63" t="s">
+      <c r="C236" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D236" s="12" t="s">
         <v>148</v>
       </c>
       <c r="E236" s="66" t="s">
@@ -6290,13 +6369,13 @@
       <c r="A237" s="40" t="n">
         <v>202</v>
       </c>
-      <c r="B237" s="63" t="n">
+      <c r="B237" s="12" t="n">
         <v>25</v>
       </c>
       <c r="C237" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D237" s="63" t="s">
+      <c r="D237" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E237" s="66" t="s">
@@ -6307,13 +6386,13 @@
       <c r="A238" s="40" t="n">
         <v>203</v>
       </c>
-      <c r="B238" s="63" t="n">
+      <c r="B238" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C238" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D238" s="63" t="s">
+      <c r="C238" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D238" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E238" s="66" t="s">
@@ -6324,13 +6403,13 @@
       <c r="A239" s="40" t="n">
         <v>204</v>
       </c>
-      <c r="B239" s="63" t="n">
+      <c r="B239" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C239" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D239" s="63" t="n">
+      <c r="D239" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E239" s="66" t="s">
@@ -6341,13 +6420,13 @@
       <c r="A240" s="40" t="n">
         <v>205</v>
       </c>
-      <c r="B240" s="63" t="n">
+      <c r="B240" s="12" t="n">
         <v>45</v>
       </c>
       <c r="C240" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D240" s="63" t="s">
+      <c r="D240" s="12" t="s">
         <v>150</v>
       </c>
       <c r="E240" s="66" t="s">
@@ -6358,13 +6437,13 @@
       <c r="A241" s="40" t="n">
         <v>206</v>
       </c>
-      <c r="B241" s="63" t="n">
+      <c r="B241" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C241" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D241" s="63" t="s">
+      <c r="C241" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D241" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E241" s="66" t="s">
@@ -6375,13 +6454,13 @@
       <c r="A242" s="40" t="n">
         <v>207</v>
       </c>
-      <c r="B242" s="63" t="n">
+      <c r="B242" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="C242" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D242" s="63" t="s">
+      <c r="C242" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D242" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E242" s="66" t="s">
@@ -6392,13 +6471,13 @@
       <c r="A243" s="40" t="n">
         <v>208</v>
       </c>
-      <c r="B243" s="63" t="n">
+      <c r="B243" s="12" t="n">
         <v>60</v>
       </c>
       <c r="C243" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D243" s="63" t="s">
+      <c r="D243" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E243" s="66" t="s">
@@ -6409,13 +6488,13 @@
       <c r="A244" s="40" t="n">
         <v>209</v>
       </c>
-      <c r="B244" s="63" t="n">
+      <c r="B244" s="12" t="n">
         <v>45</v>
       </c>
       <c r="C244" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D244" s="63" t="s">
+      <c r="D244" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E244" s="66" t="s">
@@ -6426,13 +6505,13 @@
       <c r="A245" s="40" t="n">
         <v>210</v>
       </c>
-      <c r="B245" s="63" t="n">
+      <c r="B245" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C245" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D245" s="63" t="n">
+      <c r="C245" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D245" s="12" t="n">
         <v>12</v>
       </c>
       <c r="E245" s="66" t="s">
@@ -6443,13 +6522,13 @@
       <c r="A246" s="40" t="n">
         <v>211</v>
       </c>
-      <c r="B246" s="63" t="n">
+      <c r="B246" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="C246" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D246" s="63" t="s">
+      <c r="C246" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D246" s="12" t="s">
         <v>151</v>
       </c>
       <c r="E246" s="66" t="s">
@@ -6460,13 +6539,13 @@
       <c r="A247" s="40" t="n">
         <v>212</v>
       </c>
-      <c r="B247" s="63" t="n">
+      <c r="B247" s="12" t="n">
         <v>61</v>
       </c>
       <c r="C247" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D247" s="63" t="s">
+      <c r="D247" s="12" t="s">
         <v>152</v>
       </c>
       <c r="E247" s="66" t="s">
@@ -6477,13 +6556,13 @@
       <c r="A248" s="40" t="n">
         <v>213</v>
       </c>
-      <c r="B248" s="63" t="n">
+      <c r="B248" s="12" t="n">
         <v>68</v>
       </c>
-      <c r="C248" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D248" s="63" t="n">
+      <c r="C248" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D248" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E248" s="66" t="s">
@@ -6494,13 +6573,13 @@
       <c r="A249" s="40" t="n">
         <v>214</v>
       </c>
-      <c r="B249" s="63" t="n">
+      <c r="B249" s="12" t="n">
         <v>73</v>
       </c>
       <c r="C249" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D249" s="63" t="n">
+      <c r="D249" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E249" s="66" t="s">
@@ -6511,13 +6590,13 @@
       <c r="A250" s="40" t="n">
         <v>215</v>
       </c>
-      <c r="B250" s="63" t="n">
+      <c r="B250" s="12" t="n">
         <v>33</v>
       </c>
       <c r="C250" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D250" s="63" t="s">
+      <c r="D250" s="12" t="s">
         <v>153</v>
       </c>
       <c r="E250" s="66" t="s">
@@ -6528,13 +6607,13 @@
       <c r="A251" s="40" t="n">
         <v>216</v>
       </c>
-      <c r="B251" s="63" t="n">
-        <v>57</v>
-      </c>
-      <c r="C251" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D251" s="63" t="s">
+      <c r="B251" s="12" t="n">
+        <v>57</v>
+      </c>
+      <c r="C251" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D251" s="12" t="s">
         <v>136</v>
       </c>
       <c r="E251" s="66" t="s">
@@ -6545,13 +6624,13 @@
       <c r="A252" s="40" t="n">
         <v>217</v>
       </c>
-      <c r="B252" s="63" t="n">
+      <c r="B252" s="12" t="n">
         <v>66</v>
       </c>
-      <c r="C252" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D252" s="63" t="n">
+      <c r="C252" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D252" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E252" s="66" t="s">
@@ -6562,13 +6641,13 @@
       <c r="A253" s="40" t="n">
         <v>218</v>
       </c>
-      <c r="B253" s="63" t="n">
+      <c r="B253" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="C253" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D253" s="63" t="n">
+      <c r="C253" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D253" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E253" s="66" t="s">
@@ -6579,13 +6658,13 @@
       <c r="A254" s="40" t="n">
         <v>219</v>
       </c>
-      <c r="B254" s="63" t="n">
+      <c r="B254" s="12" t="n">
         <v>42</v>
       </c>
       <c r="C254" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D254" s="63" t="n">
+      <c r="D254" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E254" s="66" t="s">
@@ -6596,13 +6675,13 @@
       <c r="A255" s="40" t="n">
         <v>220</v>
       </c>
-      <c r="B255" s="63" t="n">
+      <c r="B255" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C255" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D255" s="63" t="s">
+      <c r="D255" s="12" t="s">
         <v>115</v>
       </c>
       <c r="E255" s="66" t="s">
@@ -6613,13 +6692,13 @@
       <c r="A256" s="40" t="n">
         <v>221</v>
       </c>
-      <c r="B256" s="63" t="n">
+      <c r="B256" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C256" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D256" s="63" t="n">
+      <c r="C256" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D256" s="12" t="n">
         <v>14</v>
       </c>
       <c r="E256" s="66" t="s">
@@ -6630,13 +6709,13 @@
       <c r="A257" s="40" t="n">
         <v>222</v>
       </c>
-      <c r="B257" s="63" t="n">
+      <c r="B257" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="C257" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D257" s="63" t="s">
+      <c r="C257" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D257" s="12" t="s">
         <v>123</v>
       </c>
       <c r="E257" s="66" t="s">
@@ -6647,13 +6726,13 @@
       <c r="A258" s="40" t="n">
         <v>223</v>
       </c>
-      <c r="B258" s="63" t="n">
+      <c r="B258" s="12" t="n">
         <v>40</v>
       </c>
       <c r="C258" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D258" s="63" t="n">
+      <c r="D258" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E258" s="66" t="s">
@@ -6664,13 +6743,13 @@
       <c r="A259" s="40" t="n">
         <v>224</v>
       </c>
-      <c r="B259" s="63" t="n">
+      <c r="B259" s="12" t="n">
         <v>33</v>
       </c>
-      <c r="C259" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D259" s="63" t="s">
+      <c r="C259" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D259" s="12" t="s">
         <v>154</v>
       </c>
       <c r="E259" s="66" t="s">
@@ -6681,13 +6760,13 @@
       <c r="A260" s="40" t="n">
         <v>225</v>
       </c>
-      <c r="B260" s="63" t="n">
+      <c r="B260" s="12" t="n">
         <v>47</v>
       </c>
-      <c r="C260" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D260" s="63" t="s">
+      <c r="C260" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D260" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E260" s="66" t="s">
@@ -6698,13 +6777,13 @@
       <c r="A261" s="40" t="n">
         <v>226</v>
       </c>
-      <c r="B261" s="63" t="n">
+      <c r="B261" s="12" t="n">
         <v>39</v>
       </c>
-      <c r="C261" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D261" s="63" t="n">
+      <c r="C261" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D261" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E261" s="66" t="s">
@@ -6715,13 +6794,13 @@
       <c r="A262" s="40" t="n">
         <v>227</v>
       </c>
-      <c r="B262" s="63" t="n">
+      <c r="B262" s="12" t="n">
         <v>62</v>
       </c>
       <c r="C262" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D262" s="63" t="s">
+      <c r="D262" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E262" s="66" t="s">
@@ -6732,13 +6811,13 @@
       <c r="A263" s="40" t="n">
         <v>228</v>
       </c>
-      <c r="B263" s="63" t="n">
+      <c r="B263" s="12" t="n">
         <v>62</v>
       </c>
       <c r="C263" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D263" s="63" t="n">
+      <c r="D263" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E263" s="66" t="s">
@@ -6749,13 +6828,13 @@
       <c r="A264" s="40" t="n">
         <v>229</v>
       </c>
-      <c r="B264" s="63" t="n">
+      <c r="B264" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="C264" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D264" s="63" t="s">
+      <c r="C264" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D264" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E264" s="66" t="s">
@@ -6766,13 +6845,13 @@
       <c r="A265" s="40" t="n">
         <v>230</v>
       </c>
-      <c r="B265" s="63" t="n">
+      <c r="B265" s="12" t="n">
         <v>47</v>
       </c>
-      <c r="C265" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D265" s="63" t="n">
+      <c r="C265" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D265" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E265" s="66" t="s">
@@ -6783,13 +6862,13 @@
       <c r="A266" s="40" t="n">
         <v>231</v>
       </c>
-      <c r="B266" s="63" t="n">
+      <c r="B266" s="12" t="n">
         <v>68</v>
       </c>
       <c r="C266" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D266" s="63" t="n">
+      <c r="D266" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E266" s="66" t="s">
@@ -6800,13 +6879,13 @@
       <c r="A267" s="40" t="n">
         <v>232</v>
       </c>
-      <c r="B267" s="63" t="n">
+      <c r="B267" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C267" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D267" s="63" t="n">
+      <c r="C267" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D267" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E267" s="66" t="s">
@@ -6817,13 +6896,13 @@
       <c r="A268" s="40" t="n">
         <v>233</v>
       </c>
-      <c r="B268" s="63" t="n">
+      <c r="B268" s="12" t="n">
         <v>37</v>
       </c>
       <c r="C268" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D268" s="63" t="n">
+      <c r="D268" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E268" s="66" t="s">
@@ -6834,13 +6913,13 @@
       <c r="A269" s="40" t="n">
         <v>234</v>
       </c>
-      <c r="B269" s="63" t="n">
+      <c r="B269" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="C269" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D269" s="63" t="s">
+      <c r="C269" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D269" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E269" s="66" t="s">
@@ -6851,13 +6930,13 @@
       <c r="A270" s="40" t="n">
         <v>235</v>
       </c>
-      <c r="B270" s="63" t="n">
+      <c r="B270" s="12" t="n">
         <v>39</v>
       </c>
-      <c r="C270" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D270" s="63" t="s">
+      <c r="C270" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D270" s="12" t="s">
         <v>155</v>
       </c>
       <c r="E270" s="66" t="s">
@@ -6868,13 +6947,13 @@
       <c r="A271" s="40" t="n">
         <v>236</v>
       </c>
-      <c r="B271" s="63" t="n">
+      <c r="B271" s="12" t="n">
         <v>80</v>
       </c>
-      <c r="C271" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D271" s="63" t="n">
+      <c r="C271" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D271" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E271" s="66" t="s">
@@ -6885,13 +6964,13 @@
       <c r="A272" s="40" t="n">
         <v>237</v>
       </c>
-      <c r="B272" s="63" t="n">
+      <c r="B272" s="12" t="n">
         <v>72</v>
       </c>
       <c r="C272" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D272" s="63" t="s">
+      <c r="D272" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E272" s="66" t="s">
@@ -6902,13 +6981,13 @@
       <c r="A273" s="40" t="n">
         <v>238</v>
       </c>
-      <c r="B273" s="63" t="n">
+      <c r="B273" s="12" t="n">
         <v>64</v>
       </c>
       <c r="C273" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D273" s="63" t="n">
+      <c r="D273" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E273" s="66" t="s">
@@ -6919,13 +6998,13 @@
       <c r="A274" s="40" t="n">
         <v>239</v>
       </c>
-      <c r="B274" s="63" t="n">
+      <c r="B274" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="C274" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D274" s="63" t="s">
+      <c r="C274" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D274" s="12" t="s">
         <v>156</v>
       </c>
       <c r="E274" s="66" t="s">
@@ -6936,13 +7015,13 @@
       <c r="A275" s="40" t="n">
         <v>240</v>
       </c>
-      <c r="B275" s="63" t="n">
+      <c r="B275" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="C275" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D275" s="63" t="s">
+      <c r="C275" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D275" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E275" s="66" t="s">
@@ -6953,13 +7032,13 @@
       <c r="A276" s="40" t="n">
         <v>241</v>
       </c>
-      <c r="B276" s="63" t="n">
+      <c r="B276" s="12" t="n">
         <v>56</v>
       </c>
       <c r="C276" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D276" s="63" t="n">
+      <c r="D276" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E276" s="66" t="s">
@@ -6970,13 +7049,13 @@
       <c r="A277" s="40" t="n">
         <v>242</v>
       </c>
-      <c r="B277" s="63" t="n">
+      <c r="B277" s="12" t="n">
         <v>28</v>
       </c>
       <c r="C277" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D277" s="63" t="s">
+      <c r="D277" s="12" t="s">
         <v>138</v>
       </c>
       <c r="E277" s="66" t="s">
@@ -6987,13 +7066,13 @@
       <c r="A278" s="40" t="n">
         <v>243</v>
       </c>
-      <c r="B278" s="63" t="n">
+      <c r="B278" s="12" t="n">
         <v>56</v>
       </c>
-      <c r="C278" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D278" s="63" t="s">
+      <c r="C278" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D278" s="12" t="s">
         <v>158</v>
       </c>
       <c r="E278" s="66" t="s">
@@ -7004,13 +7083,13 @@
       <c r="A279" s="40" t="n">
         <v>244</v>
       </c>
-      <c r="B279" s="63" t="n">
+      <c r="B279" s="12" t="n">
         <v>55</v>
       </c>
       <c r="C279" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D279" s="63" t="s">
+      <c r="D279" s="12" t="s">
         <v>159</v>
       </c>
       <c r="E279" s="66" t="s">
@@ -7021,13 +7100,13 @@
       <c r="A280" s="40" t="n">
         <v>245</v>
       </c>
-      <c r="B280" s="63" t="n">
+      <c r="B280" s="12" t="n">
         <v>63</v>
       </c>
       <c r="C280" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D280" s="63" t="s">
+      <c r="D280" s="12" t="s">
         <v>160</v>
       </c>
       <c r="E280" s="66" t="s">
@@ -7038,13 +7117,13 @@
       <c r="A281" s="40" t="n">
         <v>246</v>
       </c>
-      <c r="B281" s="63" t="n">
+      <c r="B281" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C281" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D281" s="63" t="s">
+      <c r="D281" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E281" s="66" t="s">
@@ -7055,13 +7134,13 @@
       <c r="A282" s="40" t="n">
         <v>247</v>
       </c>
-      <c r="B282" s="63" t="n">
+      <c r="B282" s="12" t="n">
         <v>58</v>
       </c>
-      <c r="C282" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D282" s="63" t="s">
+      <c r="C282" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D282" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E282" s="66" t="s">
@@ -7072,13 +7151,13 @@
       <c r="A283" s="40" t="n">
         <v>248</v>
       </c>
-      <c r="B283" s="63" t="n">
+      <c r="B283" s="12" t="n">
         <v>42</v>
       </c>
-      <c r="C283" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D283" s="63" t="s">
+      <c r="C283" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D283" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E283" s="66" t="s">
@@ -7089,13 +7168,13 @@
       <c r="A284" s="40" t="n">
         <v>249</v>
       </c>
-      <c r="B284" s="63" t="n">
+      <c r="B284" s="12" t="n">
         <v>24</v>
       </c>
-      <c r="C284" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D284" s="63" t="s">
+      <c r="C284" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D284" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E284" s="66" t="s">
@@ -7106,13 +7185,13 @@
       <c r="A285" s="40" t="n">
         <v>250</v>
       </c>
-      <c r="B285" s="63" t="n">
+      <c r="B285" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="C285" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D285" s="63" t="s">
+      <c r="C285" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D285" s="12" t="s">
         <v>161</v>
       </c>
       <c r="E285" s="66" t="s">
@@ -7123,13 +7202,13 @@
       <c r="A286" s="40" t="n">
         <v>251</v>
       </c>
-      <c r="B286" s="63" t="n">
+      <c r="B286" s="12" t="n">
         <v>51</v>
       </c>
-      <c r="C286" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D286" s="63" t="n">
+      <c r="C286" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D286" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E286" s="66" t="s">
@@ -7140,13 +7219,13 @@
       <c r="A287" s="40" t="n">
         <v>252</v>
       </c>
-      <c r="B287" s="63" t="n">
+      <c r="B287" s="12" t="n">
         <v>43</v>
       </c>
-      <c r="C287" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D287" s="63" t="s">
+      <c r="C287" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D287" s="12" t="s">
         <v>162</v>
       </c>
       <c r="E287" s="66" t="s">
@@ -7157,13 +7236,13 @@
       <c r="A288" s="40" t="n">
         <v>253</v>
       </c>
-      <c r="B288" s="63" t="n">
+      <c r="B288" s="12" t="n">
         <v>67</v>
       </c>
       <c r="C288" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D288" s="63" t="s">
+      <c r="D288" s="12" t="s">
         <v>163</v>
       </c>
       <c r="E288" s="66" t="s">
@@ -7174,13 +7253,13 @@
       <c r="A289" s="40" t="n">
         <v>254</v>
       </c>
-      <c r="B289" s="63" t="n">
+      <c r="B289" s="12" t="n">
         <v>37</v>
       </c>
-      <c r="C289" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D289" s="63" t="n">
+      <c r="C289" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D289" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E289" s="66" t="s">
@@ -7191,13 +7270,13 @@
       <c r="A290" s="40" t="n">
         <v>255</v>
       </c>
-      <c r="B290" s="63" t="n">
+      <c r="B290" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="C290" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D290" s="63" t="n">
+      <c r="C290" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D290" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E290" s="66" t="s">
@@ -7208,13 +7287,13 @@
       <c r="A291" s="40" t="n">
         <v>256</v>
       </c>
-      <c r="B291" s="63" t="n">
+      <c r="B291" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="C291" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D291" s="63" t="s">
+      <c r="C291" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D291" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E291" s="66" t="s">
@@ -7225,13 +7304,13 @@
       <c r="A292" s="40" t="n">
         <v>257</v>
       </c>
-      <c r="B292" s="63" t="n">
+      <c r="B292" s="12" t="n">
         <v>45</v>
       </c>
-      <c r="C292" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D292" s="63" t="s">
+      <c r="C292" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D292" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E292" s="66" t="s">
@@ -7242,13 +7321,13 @@
       <c r="A293" s="40" t="n">
         <v>258</v>
       </c>
-      <c r="B293" s="63" t="n">
+      <c r="B293" s="12" t="n">
         <v>46</v>
       </c>
       <c r="C293" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D293" s="63" t="s">
+      <c r="D293" s="12" t="s">
         <v>164</v>
       </c>
       <c r="E293" s="66" t="s">
@@ -7259,13 +7338,13 @@
       <c r="A294" s="40" t="n">
         <v>259</v>
       </c>
-      <c r="B294" s="63" t="n">
+      <c r="B294" s="12" t="n">
         <v>32</v>
       </c>
       <c r="C294" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D294" s="63" t="s">
+      <c r="D294" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E294" s="66" t="s">
@@ -7276,13 +7355,13 @@
       <c r="A295" s="40" t="n">
         <v>260</v>
       </c>
-      <c r="B295" s="63" t="n">
+      <c r="B295" s="12" t="n">
         <v>60</v>
       </c>
       <c r="C295" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D295" s="63" t="n">
+      <c r="D295" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E295" s="66" t="s">
@@ -7293,13 +7372,13 @@
       <c r="A296" s="40" t="n">
         <v>261</v>
       </c>
-      <c r="B296" s="63" t="n">
+      <c r="B296" s="12" t="n">
         <v>49</v>
       </c>
       <c r="C296" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D296" s="63" t="s">
+      <c r="D296" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E296" s="66" t="s">
@@ -7310,13 +7389,13 @@
       <c r="A297" s="40" t="n">
         <v>262</v>
       </c>
-      <c r="B297" s="63" t="n">
+      <c r="B297" s="12" t="n">
         <v>21</v>
       </c>
       <c r="C297" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D297" s="63" t="n">
+      <c r="D297" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E297" s="66" t="s">
@@ -7327,13 +7406,13 @@
       <c r="A298" s="40" t="n">
         <v>263</v>
       </c>
-      <c r="B298" s="63" t="n">
+      <c r="B298" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="C298" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D298" s="63" t="n">
+      <c r="C298" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D298" s="12" t="n">
         <v>16</v>
       </c>
       <c r="E298" s="66" t="s">
@@ -7344,13 +7423,13 @@
       <c r="A299" s="40" t="n">
         <v>264</v>
       </c>
-      <c r="B299" s="63" t="n">
+      <c r="B299" s="12" t="n">
         <v>80</v>
       </c>
-      <c r="C299" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D299" s="63" t="s">
+      <c r="C299" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D299" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E299" s="66" t="s">
@@ -7361,13 +7440,13 @@
       <c r="A300" s="40" t="n">
         <v>265</v>
       </c>
-      <c r="B300" s="63" t="n">
+      <c r="B300" s="12" t="n">
         <v>26</v>
       </c>
-      <c r="C300" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D300" s="63" t="s">
+      <c r="C300" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D300" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E300" s="66" t="s">
@@ -7378,13 +7457,13 @@
       <c r="A301" s="40" t="n">
         <v>266</v>
       </c>
-      <c r="B301" s="63" t="n">
+      <c r="B301" s="12" t="n">
         <v>70</v>
       </c>
       <c r="C301" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D301" s="63" t="n">
+      <c r="D301" s="12" t="n">
         <v>19</v>
       </c>
       <c r="E301" s="66" t="s">
@@ -7395,13 +7474,13 @@
       <c r="A302" s="40" t="n">
         <v>267</v>
       </c>
-      <c r="B302" s="63" t="n">
+      <c r="B302" s="12" t="n">
         <v>89</v>
       </c>
       <c r="C302" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D302" s="63" t="n">
+      <c r="D302" s="12" t="n">
         <v>20</v>
       </c>
       <c r="E302" s="66" t="s">
@@ -7412,13 +7491,13 @@
       <c r="A303" s="40" t="n">
         <v>268</v>
       </c>
-      <c r="B303" s="63" t="n">
+      <c r="B303" s="12" t="n">
         <v>44</v>
       </c>
-      <c r="C303" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D303" s="63" t="s">
+      <c r="C303" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D303" s="12" t="s">
         <v>158</v>
       </c>
       <c r="E303" s="66" t="s">
@@ -7429,13 +7508,13 @@
       <c r="A304" s="40" t="n">
         <v>269</v>
       </c>
-      <c r="B304" s="63" t="n">
+      <c r="B304" s="12" t="n">
         <v>32</v>
       </c>
       <c r="C304" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D304" s="63" t="n">
+      <c r="D304" s="12" t="n">
         <v>10</v>
       </c>
       <c r="E304" s="66" t="s">
@@ -7443,19 +7522,716 @@
       </c>
     </row>
     <row r="305" spans="1:5">
-      <c r="A305" s="58" t="n">
+      <c r="A305" s="40" t="n">
         <v>270</v>
       </c>
-      <c r="B305" s="64" t="n">
+      <c r="B305" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="C305" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D305" s="64" t="n">
+      <c r="C305" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D305" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="E305" s="70" t="s">
+      <c r="E305" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" s="40" t="n">
+        <v>271</v>
+      </c>
+      <c r="B306" s="63" t="n">
+        <v>27</v>
+      </c>
+      <c r="C306" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D306" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E306" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" s="40" t="n">
+        <v>272</v>
+      </c>
+      <c r="B307" s="63" t="n">
+        <v>28</v>
+      </c>
+      <c r="C307" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D307" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E307" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" s="40" t="n">
+        <v>273</v>
+      </c>
+      <c r="B308" s="63" t="n">
+        <v>49</v>
+      </c>
+      <c r="C308" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D308" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="E308" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="A309" s="40" t="n">
+        <v>274</v>
+      </c>
+      <c r="B309" s="63" t="n">
+        <v>65</v>
+      </c>
+      <c r="C309" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D309" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E309" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5">
+      <c r="A310" s="40" t="n">
+        <v>275</v>
+      </c>
+      <c r="B310" s="63" t="n">
+        <v>63</v>
+      </c>
+      <c r="C310" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D310" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="E310" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5">
+      <c r="A311" s="40" t="n">
+        <v>276</v>
+      </c>
+      <c r="B311" s="63" t="n">
+        <v>32</v>
+      </c>
+      <c r="C311" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D311" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="E311" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5">
+      <c r="A312" s="40" t="n">
+        <v>277</v>
+      </c>
+      <c r="B312" s="63" t="n">
+        <v>80</v>
+      </c>
+      <c r="C312" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D312" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E312" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5">
+      <c r="A313" s="40" t="n">
+        <v>278</v>
+      </c>
+      <c r="B313" s="63" t="n">
+        <v>43</v>
+      </c>
+      <c r="C313" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D313" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="E313" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5">
+      <c r="A314" s="40" t="n">
+        <v>279</v>
+      </c>
+      <c r="B314" s="63" t="n">
+        <v>26</v>
+      </c>
+      <c r="C314" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D314" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E314" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5">
+      <c r="A315" s="40" t="n">
+        <v>280</v>
+      </c>
+      <c r="B315" s="63" t="n">
+        <v>28</v>
+      </c>
+      <c r="C315" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D315" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E315" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5">
+      <c r="A316" s="40" t="n">
+        <v>281</v>
+      </c>
+      <c r="B316" s="63" t="n">
+        <v>33</v>
+      </c>
+      <c r="C316" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D316" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="E316" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5">
+      <c r="A317" s="40" t="n">
+        <v>282</v>
+      </c>
+      <c r="B317" s="63" t="n">
+        <v>50</v>
+      </c>
+      <c r="C317" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D317" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="E317" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5">
+      <c r="A318" s="40" t="n">
+        <v>283</v>
+      </c>
+      <c r="B318" s="63" t="n">
+        <v>39</v>
+      </c>
+      <c r="C318" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D318" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E318" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5">
+      <c r="A319" s="40" t="n">
+        <v>284</v>
+      </c>
+      <c r="B319" s="63" t="n">
+        <v>19</v>
+      </c>
+      <c r="C319" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D319" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="E319" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5">
+      <c r="A320" s="40" t="n">
+        <v>285</v>
+      </c>
+      <c r="B320" s="63" t="n">
+        <v>64</v>
+      </c>
+      <c r="C320" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D320" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="E320" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5">
+      <c r="A321" s="40" t="n">
+        <v>286</v>
+      </c>
+      <c r="B321" s="63" t="n">
+        <v>53</v>
+      </c>
+      <c r="C321" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D321" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="E321" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5">
+      <c r="A322" s="40" t="n">
+        <v>287</v>
+      </c>
+      <c r="B322" s="63" t="n">
+        <v>29</v>
+      </c>
+      <c r="C322" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D322" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="E322" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5">
+      <c r="A323" s="40" t="n">
+        <v>288</v>
+      </c>
+      <c r="B323" s="63" t="n">
+        <v>76</v>
+      </c>
+      <c r="C323" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D323" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="E323" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
+      <c r="A324" s="40" t="n">
+        <v>289</v>
+      </c>
+      <c r="B324" s="63" t="n">
+        <v>40</v>
+      </c>
+      <c r="C324" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D324" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E324" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="A325" s="40" t="n">
+        <v>290</v>
+      </c>
+      <c r="B325" s="63" t="n">
+        <v>60</v>
+      </c>
+      <c r="C325" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D325" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E325" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5">
+      <c r="A326" s="40" t="n">
+        <v>291</v>
+      </c>
+      <c r="B326" s="63" t="n">
+        <v>71</v>
+      </c>
+      <c r="C326" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D326" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="E326" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5">
+      <c r="A327" s="40" t="n">
+        <v>292</v>
+      </c>
+      <c r="B327" s="63" t="n">
+        <v>79</v>
+      </c>
+      <c r="C327" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D327" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="E327" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
+      <c r="A328" s="40" t="n">
+        <v>293</v>
+      </c>
+      <c r="B328" s="63" t="n">
+        <v>64</v>
+      </c>
+      <c r="C328" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D328" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E328" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="A329" s="40" t="n">
+        <v>294</v>
+      </c>
+      <c r="B329" s="63" t="n">
+        <v>72</v>
+      </c>
+      <c r="C329" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D329" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="E329" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5">
+      <c r="A330" s="40" t="n">
+        <v>295</v>
+      </c>
+      <c r="B330" s="63" t="n">
+        <v>50</v>
+      </c>
+      <c r="C330" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D330" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="E330" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5">
+      <c r="A331" s="40" t="n">
+        <v>296</v>
+      </c>
+      <c r="B331" s="63" t="n">
+        <v>64</v>
+      </c>
+      <c r="C331" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D331" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E331" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5">
+      <c r="A332" s="40" t="n">
+        <v>297</v>
+      </c>
+      <c r="B332" s="63" t="n">
+        <v>47</v>
+      </c>
+      <c r="C332" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D332" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="E332" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5">
+      <c r="A333" s="40" t="n">
+        <v>298</v>
+      </c>
+      <c r="B333" s="63" t="n">
+        <v>71</v>
+      </c>
+      <c r="C333" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D333" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="E333" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
+      <c r="A334" s="40" t="n">
+        <v>299</v>
+      </c>
+      <c r="B334" s="63" t="n">
+        <v>34</v>
+      </c>
+      <c r="C334" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D334" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="E334" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5">
+      <c r="A335" s="40" t="n">
+        <v>300</v>
+      </c>
+      <c r="B335" s="63" t="n">
+        <v>63</v>
+      </c>
+      <c r="C335" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D335" s="63" t="n">
+        <v>21</v>
+      </c>
+      <c r="E335" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
+      <c r="A336" s="40" t="n">
+        <v>301</v>
+      </c>
+      <c r="B336" s="63" t="n">
+        <v>42</v>
+      </c>
+      <c r="C336" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D336" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="E336" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5">
+      <c r="A337" s="40" t="n">
+        <v>302</v>
+      </c>
+      <c r="B337" s="63" t="n">
+        <v>55</v>
+      </c>
+      <c r="C337" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D337" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E337" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5">
+      <c r="A338" s="40" t="n">
+        <v>303</v>
+      </c>
+      <c r="B338" s="63" t="n">
+        <v>33</v>
+      </c>
+      <c r="C338" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D338" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="E338" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5">
+      <c r="A339" s="40" t="n">
+        <v>304</v>
+      </c>
+      <c r="B339" s="63" t="n">
+        <v>73</v>
+      </c>
+      <c r="C339" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D339" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="E339" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5">
+      <c r="A340" s="40" t="n">
+        <v>305</v>
+      </c>
+      <c r="B340" s="63" t="n">
+        <v>49</v>
+      </c>
+      <c r="C340" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D340" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="E340" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5">
+      <c r="A341" s="40" t="n">
+        <v>306</v>
+      </c>
+      <c r="B341" s="63" t="n">
+        <v>67</v>
+      </c>
+      <c r="C341" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D341" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="E341" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5">
+      <c r="A342" s="40" t="n">
+        <v>307</v>
+      </c>
+      <c r="B342" s="63" t="n">
+        <v>30</v>
+      </c>
+      <c r="C342" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D342" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="E342" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5">
+      <c r="A343" s="40" t="n">
+        <v>308</v>
+      </c>
+      <c r="B343" s="63" t="n">
+        <v>30</v>
+      </c>
+      <c r="C343" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D343" s="63" t="n">
+        <v>21</v>
+      </c>
+      <c r="E343" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5">
+      <c r="A344" s="40" t="n">
+        <v>309</v>
+      </c>
+      <c r="B344" s="63" t="n">
+        <v>44</v>
+      </c>
+      <c r="C344" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D344" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E344" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5">
+      <c r="A345" s="40" t="n">
+        <v>310</v>
+      </c>
+      <c r="B345" s="63" t="n">
+        <v>65</v>
+      </c>
+      <c r="C345" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D345" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="E345" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5">
+      <c r="A346" s="58" t="n">
+        <v>311</v>
+      </c>
+      <c r="B346" s="64" t="n">
+        <v>52</v>
+      </c>
+      <c r="C346" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D346" s="64" t="n">
+        <v>21</v>
+      </c>
+      <c r="E346" s="70" t="s">
         <v>54</v>
       </c>
     </row>
@@ -7469,7 +8245,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1588791772" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1588954570" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -7478,16 +8254,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1588791772" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1588791772" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1588791772" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1588791772" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1588954570" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1588954570" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1588954570" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1588954570" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1588791772" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1588954570" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Adição de 10 novos pacientes
</commit_message>
<xml_diff>
--- a/SINTOMAS CORONAVIRUS.xlsx
+++ b/SINTOMAS CORONAVIRUS.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1588954570" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1588954570" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1588954570" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1588954570"/>
+      <pm:revision xmlns:pm="smNativeData" day="1589227222" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1589227222" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1589227222" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1589227222"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="197">
   <si>
     <t>CORONAVIRUS</t>
   </si>
@@ -596,6 +596,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 12, 20, 21, 26</t>
+  </si>
+  <si>
+    <t>10, 16, 18</t>
+  </si>
+  <si>
+    <t>10, 11, 15, 18,  23</t>
+  </si>
+  <si>
+    <t>15, 21</t>
+  </si>
+  <si>
+    <t>14, 18, 23</t>
+  </si>
+  <si>
+    <t>11, 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14, 20, 21 </t>
   </si>
 </sst>
 </file>
@@ -620,7 +638,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1588954570" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1589227222" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -636,7 +654,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1588954570" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1589227222" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -670,7 +688,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -681,7 +699,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -692,7 +710,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -703,7 +721,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -717,7 +735,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -734,7 +752,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="12" fgClr="0000FF00" bgLvl="88" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -757,7 +775,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -768,7 +786,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -779,7 +797,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -802,7 +820,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -813,7 +831,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -851,7 +869,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -862,7 +880,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -879,7 +897,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1588954570" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589227222" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -919,7 +937,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570"/>
+          <pm:border xmlns:pm="smNativeData" id="1589227222"/>
         </ext>
       </extLst>
     </border>
@@ -938,7 +956,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -962,7 +980,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -986,7 +1004,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1009,7 +1027,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1031,7 +1049,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1055,7 +1073,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1079,7 +1097,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1103,7 +1121,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1127,7 +1145,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1150,7 +1168,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1174,7 +1192,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1197,7 +1215,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1221,7 +1239,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1245,7 +1263,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1268,7 +1286,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1292,7 +1310,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1316,7 +1334,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1340,7 +1358,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1363,7 +1381,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1386,7 +1404,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1409,7 +1427,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1433,7 +1451,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1457,7 +1475,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1481,7 +1499,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1504,7 +1522,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1527,7 +1545,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1550,7 +1568,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1573,7 +1591,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1594,7 +1612,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1617,7 +1635,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1641,7 +1659,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1665,7 +1683,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1688,7 +1706,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1710,7 +1728,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1733,7 +1751,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1757,7 +1775,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1780,7 +1798,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
@@ -1803,7 +1821,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1826,7 +1844,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1848,7 +1866,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570"/>
+          <pm:border xmlns:pm="smNativeData" id="1589227222"/>
         </ext>
       </extLst>
     </border>
@@ -1867,7 +1885,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1889,7 +1907,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1910,7 +1928,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1931,7 +1949,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1953,7 +1971,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1974,7 +1992,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1588954570">
+          <pm:border xmlns:pm="smNativeData" id="1589227222">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -2186,10 +2204,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1588954570" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1589227222" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1588954570" count="4">
+      <pm:colors xmlns:pm="smNativeData" id="1589227222" count="4">
         <pm:color name="Color 24" rgb="FFFF9E"/>
         <pm:color name="Color 25" rgb="FF9E9E"/>
         <pm:color name="Color 26" rgb="FFFFE0"/>
@@ -2456,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H346"/>
+  <dimension ref="A1:H356"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="F338" sqref="F338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -7542,13 +7560,13 @@
       <c r="A306" s="40" t="n">
         <v>271</v>
       </c>
-      <c r="B306" s="63" t="n">
+      <c r="B306" s="12" t="n">
         <v>27</v>
       </c>
       <c r="C306" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D306" s="63" t="s">
+      <c r="D306" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E306" s="66" t="s">
@@ -7559,13 +7577,13 @@
       <c r="A307" s="40" t="n">
         <v>272</v>
       </c>
-      <c r="B307" s="63" t="n">
+      <c r="B307" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="C307" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D307" s="63" t="s">
+      <c r="C307" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D307" s="12" t="s">
         <v>165</v>
       </c>
       <c r="E307" s="66" t="s">
@@ -7576,13 +7594,13 @@
       <c r="A308" s="40" t="n">
         <v>273</v>
       </c>
-      <c r="B308" s="63" t="n">
+      <c r="B308" s="12" t="n">
         <v>49</v>
       </c>
       <c r="C308" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D308" s="63" t="s">
+      <c r="D308" s="12" t="s">
         <v>166</v>
       </c>
       <c r="E308" s="66" t="s">
@@ -7593,13 +7611,13 @@
       <c r="A309" s="40" t="n">
         <v>274</v>
       </c>
-      <c r="B309" s="63" t="n">
+      <c r="B309" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C309" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D309" s="63" t="s">
+      <c r="D309" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E309" s="66" t="s">
@@ -7610,13 +7628,13 @@
       <c r="A310" s="40" t="n">
         <v>275</v>
       </c>
-      <c r="B310" s="63" t="n">
+      <c r="B310" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="C310" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D310" s="63" t="s">
+      <c r="C310" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D310" s="12" t="s">
         <v>167</v>
       </c>
       <c r="E310" s="66" t="s">
@@ -7627,13 +7645,13 @@
       <c r="A311" s="40" t="n">
         <v>276</v>
       </c>
-      <c r="B311" s="63" t="n">
+      <c r="B311" s="12" t="n">
         <v>32</v>
       </c>
       <c r="C311" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D311" s="63" t="s">
+      <c r="D311" s="12" t="s">
         <v>168</v>
       </c>
       <c r="E311" s="66" t="s">
@@ -7644,13 +7662,13 @@
       <c r="A312" s="40" t="n">
         <v>277</v>
       </c>
-      <c r="B312" s="63" t="n">
+      <c r="B312" s="12" t="n">
         <v>80</v>
       </c>
-      <c r="C312" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D312" s="63" t="s">
+      <c r="C312" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D312" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E312" s="66" t="s">
@@ -7661,13 +7679,13 @@
       <c r="A313" s="40" t="n">
         <v>278</v>
       </c>
-      <c r="B313" s="63" t="n">
+      <c r="B313" s="12" t="n">
         <v>43</v>
       </c>
-      <c r="C313" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D313" s="63" t="s">
+      <c r="C313" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D313" s="12" t="s">
         <v>169</v>
       </c>
       <c r="E313" s="66" t="s">
@@ -7678,13 +7696,13 @@
       <c r="A314" s="40" t="n">
         <v>279</v>
       </c>
-      <c r="B314" s="63" t="n">
+      <c r="B314" s="12" t="n">
         <v>26</v>
       </c>
       <c r="C314" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D314" s="63" t="s">
+      <c r="D314" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E314" s="66" t="s">
@@ -7695,13 +7713,13 @@
       <c r="A315" s="40" t="n">
         <v>280</v>
       </c>
-      <c r="B315" s="63" t="n">
+      <c r="B315" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="C315" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D315" s="63" t="s">
+      <c r="C315" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D315" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E315" s="66" t="s">
@@ -7712,13 +7730,13 @@
       <c r="A316" s="40" t="n">
         <v>281</v>
       </c>
-      <c r="B316" s="63" t="n">
+      <c r="B316" s="12" t="n">
         <v>33</v>
       </c>
-      <c r="C316" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D316" s="63" t="s">
+      <c r="C316" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D316" s="12" t="s">
         <v>170</v>
       </c>
       <c r="E316" s="66" t="s">
@@ -7729,13 +7747,13 @@
       <c r="A317" s="40" t="n">
         <v>282</v>
       </c>
-      <c r="B317" s="63" t="n">
+      <c r="B317" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C317" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D317" s="63" t="s">
+      <c r="C317" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D317" s="12" t="s">
         <v>168</v>
       </c>
       <c r="E317" s="66" t="s">
@@ -7746,13 +7764,13 @@
       <c r="A318" s="40" t="n">
         <v>283</v>
       </c>
-      <c r="B318" s="63" t="n">
+      <c r="B318" s="12" t="n">
         <v>39</v>
       </c>
       <c r="C318" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D318" s="63" t="s">
+      <c r="D318" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E318" s="66" t="s">
@@ -7763,13 +7781,13 @@
       <c r="A319" s="40" t="n">
         <v>284</v>
       </c>
-      <c r="B319" s="63" t="n">
+      <c r="B319" s="12" t="n">
         <v>19</v>
       </c>
       <c r="C319" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D319" s="63" t="s">
+      <c r="D319" s="12" t="s">
         <v>171</v>
       </c>
       <c r="E319" s="66" t="s">
@@ -7780,13 +7798,13 @@
       <c r="A320" s="40" t="n">
         <v>285</v>
       </c>
-      <c r="B320" s="63" t="n">
+      <c r="B320" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C320" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D320" s="63" t="s">
+      <c r="C320" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D320" s="12" t="s">
         <v>172</v>
       </c>
       <c r="E320" s="66" t="s">
@@ -7797,13 +7815,13 @@
       <c r="A321" s="40" t="n">
         <v>286</v>
       </c>
-      <c r="B321" s="63" t="n">
+      <c r="B321" s="12" t="n">
         <v>53</v>
       </c>
-      <c r="C321" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D321" s="63" t="s">
+      <c r="C321" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D321" s="12" t="s">
         <v>173</v>
       </c>
       <c r="E321" s="66" t="s">
@@ -7814,13 +7832,13 @@
       <c r="A322" s="40" t="n">
         <v>287</v>
       </c>
-      <c r="B322" s="63" t="n">
+      <c r="B322" s="12" t="n">
         <v>29</v>
       </c>
-      <c r="C322" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D322" s="63" t="s">
+      <c r="C322" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D322" s="12" t="s">
         <v>174</v>
       </c>
       <c r="E322" s="66" t="s">
@@ -7831,13 +7849,13 @@
       <c r="A323" s="40" t="n">
         <v>288</v>
       </c>
-      <c r="B323" s="63" t="n">
+      <c r="B323" s="12" t="n">
         <v>76</v>
       </c>
       <c r="C323" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D323" s="63" t="s">
+      <c r="D323" s="12" t="s">
         <v>175</v>
       </c>
       <c r="E323" s="66" t="s">
@@ -7848,13 +7866,13 @@
       <c r="A324" s="40" t="n">
         <v>289</v>
       </c>
-      <c r="B324" s="63" t="n">
+      <c r="B324" s="12" t="n">
         <v>40</v>
       </c>
       <c r="C324" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D324" s="63" t="s">
+      <c r="D324" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E324" s="66" t="s">
@@ -7865,13 +7883,13 @@
       <c r="A325" s="40" t="n">
         <v>290</v>
       </c>
-      <c r="B325" s="63" t="n">
+      <c r="B325" s="12" t="n">
         <v>60</v>
       </c>
       <c r="C325" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D325" s="63" t="s">
+      <c r="D325" s="12" t="s">
         <v>176</v>
       </c>
       <c r="E325" s="66" t="s">
@@ -7882,13 +7900,13 @@
       <c r="A326" s="40" t="n">
         <v>291</v>
       </c>
-      <c r="B326" s="63" t="n">
+      <c r="B326" s="12" t="n">
         <v>71</v>
       </c>
-      <c r="C326" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D326" s="63" t="s">
+      <c r="C326" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D326" s="12" t="s">
         <v>177</v>
       </c>
       <c r="E326" s="66" t="s">
@@ -7899,13 +7917,13 @@
       <c r="A327" s="40" t="n">
         <v>292</v>
       </c>
-      <c r="B327" s="63" t="n">
+      <c r="B327" s="12" t="n">
         <v>79</v>
       </c>
       <c r="C327" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D327" s="63" t="s">
+      <c r="D327" s="12" t="s">
         <v>178</v>
       </c>
       <c r="E327" s="66" t="s">
@@ -7916,13 +7934,13 @@
       <c r="A328" s="40" t="n">
         <v>293</v>
       </c>
-      <c r="B328" s="63" t="n">
+      <c r="B328" s="12" t="n">
         <v>64</v>
       </c>
       <c r="C328" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D328" s="63" t="s">
+      <c r="D328" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E328" s="66" t="s">
@@ -7933,13 +7951,13 @@
       <c r="A329" s="40" t="n">
         <v>294</v>
       </c>
-      <c r="B329" s="63" t="n">
+      <c r="B329" s="12" t="n">
         <v>72</v>
       </c>
-      <c r="C329" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D329" s="63" t="s">
+      <c r="C329" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D329" s="12" t="s">
         <v>179</v>
       </c>
       <c r="E329" s="66" t="s">
@@ -7950,13 +7968,13 @@
       <c r="A330" s="40" t="n">
         <v>295</v>
       </c>
-      <c r="B330" s="63" t="n">
+      <c r="B330" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C330" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D330" s="63" t="s">
+      <c r="C330" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D330" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E330" s="66" t="s">
@@ -7967,13 +7985,13 @@
       <c r="A331" s="40" t="n">
         <v>296</v>
       </c>
-      <c r="B331" s="63" t="n">
+      <c r="B331" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C331" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D331" s="63" t="s">
+      <c r="C331" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D331" s="12" t="s">
         <v>181</v>
       </c>
       <c r="E331" s="66" t="s">
@@ -7984,13 +8002,13 @@
       <c r="A332" s="40" t="n">
         <v>297</v>
       </c>
-      <c r="B332" s="63" t="n">
+      <c r="B332" s="12" t="n">
         <v>47</v>
       </c>
       <c r="C332" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D332" s="63" t="s">
+      <c r="D332" s="12" t="s">
         <v>182</v>
       </c>
       <c r="E332" s="66" t="s">
@@ -8001,13 +8019,13 @@
       <c r="A333" s="40" t="n">
         <v>298</v>
       </c>
-      <c r="B333" s="63" t="n">
+      <c r="B333" s="12" t="n">
         <v>71</v>
       </c>
       <c r="C333" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D333" s="63" t="s">
+      <c r="D333" s="12" t="s">
         <v>183</v>
       </c>
       <c r="E333" s="66" t="s">
@@ -8018,13 +8036,13 @@
       <c r="A334" s="40" t="n">
         <v>299</v>
       </c>
-      <c r="B334" s="63" t="n">
+      <c r="B334" s="12" t="n">
         <v>34</v>
       </c>
       <c r="C334" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D334" s="63" t="s">
+      <c r="D334" s="12" t="s">
         <v>184</v>
       </c>
       <c r="E334" s="66" t="s">
@@ -8035,13 +8053,13 @@
       <c r="A335" s="40" t="n">
         <v>300</v>
       </c>
-      <c r="B335" s="63" t="n">
+      <c r="B335" s="12" t="n">
         <v>63</v>
       </c>
       <c r="C335" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D335" s="63" t="n">
+      <c r="D335" s="12" t="n">
         <v>21</v>
       </c>
       <c r="E335" s="66" t="s">
@@ -8052,13 +8070,13 @@
       <c r="A336" s="40" t="n">
         <v>301</v>
       </c>
-      <c r="B336" s="63" t="n">
+      <c r="B336" s="12" t="n">
         <v>42</v>
       </c>
-      <c r="C336" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D336" s="63" t="s">
+      <c r="C336" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D336" s="12" t="s">
         <v>185</v>
       </c>
       <c r="E336" s="66" t="s">
@@ -8069,13 +8087,13 @@
       <c r="A337" s="40" t="n">
         <v>302</v>
       </c>
-      <c r="B337" s="63" t="n">
+      <c r="B337" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="C337" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D337" s="63" t="s">
+      <c r="C337" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D337" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E337" s="66" t="s">
@@ -8086,13 +8104,13 @@
       <c r="A338" s="40" t="n">
         <v>303</v>
       </c>
-      <c r="B338" s="63" t="n">
+      <c r="B338" s="12" t="n">
         <v>33</v>
       </c>
-      <c r="C338" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D338" s="63" t="s">
+      <c r="C338" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D338" s="12" t="s">
         <v>186</v>
       </c>
       <c r="E338" s="66" t="s">
@@ -8103,13 +8121,13 @@
       <c r="A339" s="40" t="n">
         <v>304</v>
       </c>
-      <c r="B339" s="63" t="n">
+      <c r="B339" s="12" t="n">
         <v>73</v>
       </c>
       <c r="C339" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D339" s="63" t="s">
+      <c r="D339" s="12" t="s">
         <v>185</v>
       </c>
       <c r="E339" s="66" t="s">
@@ -8120,13 +8138,13 @@
       <c r="A340" s="40" t="n">
         <v>305</v>
       </c>
-      <c r="B340" s="63" t="n">
+      <c r="B340" s="12" t="n">
         <v>49</v>
       </c>
-      <c r="C340" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D340" s="63" t="s">
+      <c r="C340" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D340" s="12" t="s">
         <v>187</v>
       </c>
       <c r="E340" s="66" t="s">
@@ -8137,13 +8155,13 @@
       <c r="A341" s="40" t="n">
         <v>306</v>
       </c>
-      <c r="B341" s="63" t="n">
+      <c r="B341" s="12" t="n">
         <v>67</v>
       </c>
-      <c r="C341" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D341" s="63" t="s">
+      <c r="C341" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D341" s="12" t="s">
         <v>188</v>
       </c>
       <c r="E341" s="66" t="s">
@@ -8154,13 +8172,13 @@
       <c r="A342" s="40" t="n">
         <v>307</v>
       </c>
-      <c r="B342" s="63" t="n">
+      <c r="B342" s="12" t="n">
         <v>30</v>
       </c>
       <c r="C342" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D342" s="63" t="s">
+      <c r="D342" s="12" t="s">
         <v>189</v>
       </c>
       <c r="E342" s="66" t="s">
@@ -8171,13 +8189,13 @@
       <c r="A343" s="40" t="n">
         <v>308</v>
       </c>
-      <c r="B343" s="63" t="n">
+      <c r="B343" s="12" t="n">
         <v>30</v>
       </c>
       <c r="C343" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D343" s="63" t="n">
+      <c r="D343" s="12" t="n">
         <v>21</v>
       </c>
       <c r="E343" s="66" t="s">
@@ -8188,13 +8206,13 @@
       <c r="A344" s="40" t="n">
         <v>309</v>
       </c>
-      <c r="B344" s="63" t="n">
+      <c r="B344" s="12" t="n">
         <v>44</v>
       </c>
-      <c r="C344" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D344" s="63" t="s">
+      <c r="C344" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D344" s="12" t="s">
         <v>190</v>
       </c>
       <c r="E344" s="66" t="s">
@@ -8205,13 +8223,13 @@
       <c r="A345" s="40" t="n">
         <v>310</v>
       </c>
-      <c r="B345" s="63" t="n">
+      <c r="B345" s="12" t="n">
         <v>65</v>
       </c>
       <c r="C345" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D345" s="63" t="s">
+      <c r="D345" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E345" s="66" t="s">
@@ -8219,19 +8237,189 @@
       </c>
     </row>
     <row r="346" spans="1:5">
-      <c r="A346" s="58" t="n">
+      <c r="A346" s="40" t="n">
         <v>311</v>
       </c>
-      <c r="B346" s="64" t="n">
-        <v>52</v>
-      </c>
-      <c r="C346" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="D346" s="64" t="n">
+      <c r="B346" s="12" t="n">
+        <v>52</v>
+      </c>
+      <c r="C346" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D346" s="12" t="n">
         <v>21</v>
       </c>
-      <c r="E346" s="70" t="s">
+      <c r="E346" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5">
+      <c r="A347" s="40" t="n">
+        <v>312</v>
+      </c>
+      <c r="B347" s="63" t="n">
+        <v>52</v>
+      </c>
+      <c r="C347" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D347" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E347" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5">
+      <c r="A348" s="40" t="n">
+        <v>313</v>
+      </c>
+      <c r="B348" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C348" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D348" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="E348" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5">
+      <c r="A349" s="40" t="n">
+        <v>314</v>
+      </c>
+      <c r="B349" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C349" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="D349" s="63" t="s">
+        <v>192</v>
+      </c>
+      <c r="E349" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5">
+      <c r="A350" s="40" t="n">
+        <v>315</v>
+      </c>
+      <c r="B350" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C350" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D350" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="E350" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5">
+      <c r="A351" s="40" t="n">
+        <v>316</v>
+      </c>
+      <c r="B351" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C351" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D351" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="E351" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5">
+      <c r="A352" s="40" t="n">
+        <v>317</v>
+      </c>
+      <c r="B352" s="63" t="n">
+        <v>44</v>
+      </c>
+      <c r="C352" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D352" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="E352" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5">
+      <c r="A353" s="40" t="n">
+        <v>318</v>
+      </c>
+      <c r="B353" s="63" t="n">
+        <v>33</v>
+      </c>
+      <c r="C353" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D353" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="E353" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5">
+      <c r="A354" s="40" t="n">
+        <v>319</v>
+      </c>
+      <c r="B354" s="63" t="n">
+        <v>29</v>
+      </c>
+      <c r="C354" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D354" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E354" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5">
+      <c r="A355" s="40" t="n">
+        <v>320</v>
+      </c>
+      <c r="B355" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C355" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D355" s="63" t="s">
+        <v>195</v>
+      </c>
+      <c r="E355" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5">
+      <c r="A356" s="58" t="n">
+        <v>321</v>
+      </c>
+      <c r="B356" s="64" t="n">
+        <v>72</v>
+      </c>
+      <c r="C356" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D356" s="64" t="s">
+        <v>196</v>
+      </c>
+      <c r="E356" s="70" t="s">
         <v>54</v>
       </c>
     </row>
@@ -8245,7 +8433,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1588954570" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1589227222" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -8254,16 +8442,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1588954570" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1588954570" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1588954570" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1588954570" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1589227222" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1589227222" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1589227222" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1589227222" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1588954570" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1589227222" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>